<commit_message>
Okay now NR is done with one iteration. just need to add v and t updates and then check convergence. then check if the p or q should be negative if its generating or whatever
</commit_message>
<xml_diff>
--- a/ex_nr.xlsx
+++ b/ex_nr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracedepietro/Desktop/4205/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracedepietro/Desktop/4205/project/PowerFlow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2046182B-3531-F54A-B598-2A08E43BD7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9608DC-E3DE-8E40-83C7-D2B55054F079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13080" yWindow="500" windowWidth="20920" windowHeight="14340" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
+    <workbookView xWindow="4680" yWindow="500" windowWidth="20920" windowHeight="14340" activeTab="1" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CC4DDF-8E3E-324E-AB44-8876A263AA5F}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,10 +460,16 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1.05</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -474,10 +480,16 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>1.04</v>
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>0.5</v>
+      </c>
+      <c r="F3">
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -487,11 +499,11 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4">
-        <v>1.5</v>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -503,8 +515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3C53D1-2A7C-F44F-B86A-DD1711AAE24B}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,10 +537,10 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C2">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -539,7 +551,7 @@
         <v>0.05</v>
       </c>
       <c r="C3">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -547,10 +559,10 @@
         <v>23</v>
       </c>
       <c r="B4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.05</v>
       </c>
       <c r="C4">
-        <v>0.1</v>
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved NR methods to a function so main file is clear. Implemented working Cutsem Ybus.
</commit_message>
<xml_diff>
--- a/ex_nr.xlsx
+++ b/ex_nr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracedepietro/Desktop/4205/project/PowerFlow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9608DC-E3DE-8E40-83C7-D2B55054F079}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC80F2AE-D93D-D04D-B559-8AA945A7A4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4680" yWindow="500" windowWidth="20920" windowHeight="14340" activeTab="1" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>bus_num</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>shunt_r</t>
+  </si>
+  <si>
+    <t>shunt_x</t>
   </si>
 </sst>
 </file>
@@ -513,15 +519,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3C53D1-2A7C-F44F-B86A-DD1711AAE24B}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -531,8 +537,14 @@
       <c r="C1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>12</v>
       </c>
@@ -542,8 +554,14 @@
       <c r="C2">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>13</v>
       </c>
@@ -553,8 +571,14 @@
       <c r="C3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>23</v>
       </c>
@@ -563,6 +587,12 @@
       </c>
       <c r="C4">
         <v>0.15</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Iterate method finsihed and goes until the convergence criteria is met
</commit_message>
<xml_diff>
--- a/ex_nr.xlsx
+++ b/ex_nr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracedepietro/Desktop/4205/project/PowerFlow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC80F2AE-D93D-D04D-B559-8AA945A7A4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C181BFFD-E710-4445-B48F-5F939CEA1C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="500" windowWidth="20920" windowHeight="14340" activeTab="1" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
+    <workbookView xWindow="4680" yWindow="500" windowWidth="20920" windowHeight="14340" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -432,8 +432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CC4DDF-8E3E-324E-AB44-8876A263AA5F}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -472,10 +472,10 @@
         <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -492,10 +492,10 @@
         <v>0</v>
       </c>
       <c r="E3">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -521,7 +521,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3C53D1-2A7C-F44F-B86A-DD1711AAE24B}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
changed decoupled load flow to use less copy pasting
</commit_message>
<xml_diff>
--- a/ex_nr.xlsx
+++ b/ex_nr.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracedepietro/Desktop/4205/project/PowerFlow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C181BFFD-E710-4445-B48F-5F939CEA1C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292F39C6-8BE6-9A43-B3AA-94B5D786697F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="500" windowWidth="20920" windowHeight="14340" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
+    <workbookView xWindow="4680" yWindow="500" windowWidth="20920" windowHeight="14340" activeTab="1" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>bus_num</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>shunt_x</t>
+  </si>
+  <si>
+    <t>t_x</t>
+  </si>
+  <si>
+    <t>t_a</t>
   </si>
 </sst>
 </file>
@@ -432,7 +438,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CC4DDF-8E3E-324E-AB44-8876A263AA5F}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
@@ -519,15 +525,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3C53D1-2A7C-F44F-B86A-DD1711AAE24B}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -543,8 +549,14 @@
       <c r="E1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>12</v>
       </c>
@@ -561,7 +573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>13</v>
       </c>
@@ -578,7 +590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
FDLF Q constrains - start
</commit_message>
<xml_diff>
--- a/ex_nr.xlsx
+++ b/ex_nr.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracedepietro/Desktop/4205/project/PowerFlow/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ximena\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292F39C6-8BE6-9A43-B3AA-94B5D786697F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179C92B9-01DB-456C-A273-E6500CE15BB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="500" windowWidth="20920" windowHeight="14340" activeTab="1" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
+    <workbookView xWindow="1900" yWindow="1900" windowWidth="13290" windowHeight="8430" xr2:uid="{4767C10A-D1AC-5641-9DB1-56441DD8E711}"/>
   </bookViews>
   <sheets>
     <sheet name="initial" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>bus_num</t>
   </si>
@@ -48,43 +48,46 @@
     <t>slack</t>
   </si>
   <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>line</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>shunt_r</t>
+  </si>
+  <si>
+    <t>shunt_x</t>
+  </si>
+  <si>
     <t>pv</t>
   </si>
   <si>
     <t>pq</t>
   </si>
   <si>
-    <t>V</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Q</t>
-  </si>
-  <si>
-    <t>line</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>shunt_r</t>
-  </si>
-  <si>
-    <t>shunt_x</t>
-  </si>
-  <si>
     <t>t_x</t>
   </si>
   <si>
     <t>t_a</t>
+  </si>
+  <si>
+    <t>q_lim</t>
   </si>
 </sst>
 </file>
@@ -436,15 +439,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99CC4DDF-8E3E-324E-AB44-8876A263AA5F}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -452,19 +455,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -472,50 +478,38 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>1.05</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2">
-        <v>-1</v>
-      </c>
-      <c r="F2">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E3">
-        <v>-0.5</v>
+        <v>-4</v>
       </c>
       <c r="F3">
-        <v>-0.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>-2.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
+        <v>1.04</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -527,27 +521,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3C53D1-2A7C-F44F-B86A-DD1711AAE24B}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
       </c>
       <c r="F1" t="s">
         <v>14</v>
@@ -556,15 +550,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>12</v>
       </c>
       <c r="B2">
-        <v>0.05</v>
+        <v>0.02</v>
       </c>
       <c r="C2">
-        <v>0.2</v>
+        <v>0.04</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -573,15 +567,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>13</v>
       </c>
       <c r="B3">
-        <v>0.05</v>
+        <v>0.01</v>
       </c>
       <c r="C3">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -590,15 +584,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>23</v>
       </c>
       <c r="B4">
-        <v>0.05</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="C4">
-        <v>0.15</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="D4">
         <v>0</v>

</xml_diff>